<commit_message>
I add a feature that have a multi-language function, which can choose the language the company use for their business in large probability.
</commit_message>
<xml_diff>
--- a/data/input/companies.xlsx
+++ b/data/input/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6777DCFB-0D2E-4B44-8490-BF91DC886FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD81B30B-C392-F44B-B4FA-F4F172E17EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Process</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>es</t>
   </si>
 </sst>
 </file>
@@ -271,23 +277,23 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,7 +632,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -634,9 +640,10 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="31.875" customWidth="1"/>
     <col min="4" max="4" width="26.875" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -652,8 +659,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -670,9 +680,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -686,8 +696,11 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -704,7 +717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -721,7 +734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -738,7 +751,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -755,7 +768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -772,7 +785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -789,129 +802,129 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2"/>
-      <c r="C45" s="8"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="2"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="7"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
-      <c r="C48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -961,12 +974,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C51:C60"/>
-    <mergeCell ref="B51:B60"/>
     <mergeCell ref="B33:B42"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="B43:B44"/>
@@ -975,6 +982,12 @@
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C51:C60"/>
+    <mergeCell ref="B51:B60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Refactored with multi-language support including email TLD check.
</commit_message>
<xml_diff>
--- a/data/input/companies.xlsx
+++ b/data/input/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD81B30B-C392-F44B-B4FA-F4F172E17EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F758BC-9A4D-0B49-803D-19D229B2C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Process</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>es</t>
+  </si>
+  <si>
+    <t>de</t>
   </si>
 </sst>
 </file>
@@ -631,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -716,6 +719,9 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -732,6 +738,9 @@
       </c>
       <c r="E5" t="s">
         <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update to make the saved excel to dispaly full column header names when saving processed data to the excel.
</commit_message>
<xml_diff>
--- a/data/input/companies.xlsx
+++ b/data/input/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F758BC-9A4D-0B49-803D-19D229B2C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EE609B-9AF9-1A4C-8C8F-E33B4FF099AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Process</t>
   </si>
@@ -51,56 +51,6 @@
   </si>
   <si>
     <t>John Chen</t>
-  </si>
-  <si>
-    <t>2025/03/15 10:12</t>
-  </si>
-  <si>
-    <t>https://www.google.com</t>
-  </si>
-  <si>
-    <t>Google is a technology company that specializes in internet-related services and products, including search engines, online advertising technologies, cloud computing, software, and hardware. Its primary activity is organizing the world's information and making it universally accessible and useful through its search engine and various other digital services.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Dear John Chen,&lt;/p&gt;
-&lt;p&gt;I hope this message finds you well. My name is Jimmy, and I am the Overseas Sales Manager at &lt;strong&gt;Skyfend&lt;/strong&gt;, a subsidiary of Autel. We have been closely following Google’s remarkable advancements and believe there is significant potential for collaboration between our companies.&lt;/p&gt;
-&lt;p&gt;Skyfend has established a strong global presence, exporting advanced counter-drone devices to partners across Africa, Europe, and America. Our solutions, such as the &lt;strong&gt;Tracer&lt;/strong&gt; and &lt;strong&gt;Defender&lt;/strong&gt; systems, are designed to address FPV drone threats and ensure the security of commercial drones like DJI, Autel, and Parrot.&lt;/p&gt;
-&lt;p&gt;I would like to propose a strategic partnership to explore the following cooperation opportunities:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;&lt;strong&gt;AI/ML-Enhanced Drone Threat Detection &amp; Prediction:&lt;/strong&gt; Integrating Google’s AI/ML tools with Skyfend’s detection systems to improve accuracy and predict intrusion patterns.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Cloud-Based Command &amp; Control Infrastructure:&lt;/strong&gt; Hosting Skyfend’s Guider C2 software on Google Cloud for scalable, real-time analytics.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Secure Airspace Solutions for Google Wing Drone Deliveries:&lt;/strong&gt; Protecting delivery drones with Skyfend’s portable jammers and spoofers.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Geospatial Threat Mapping with Google Earth/Maps:&lt;/strong&gt; Visualizing real-time drone threats using Google’s geospatial APIs.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;IoT-Enabled Security Ecosystems:&lt;/strong&gt; Combining Skyfend’s detectors with Google Nest or Android platforms for smart perimeter security.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;I have attached a product brochure for your reference. I would be delighted to schedule a video meeting or call to discuss these opportunities further. Please let me know your availability.&lt;/p&gt;
-&lt;p&gt;Looking forward to your response.&lt;/p&gt;
-&lt;p&gt;Best regards,&lt;br&gt;Jimmy&lt;br&gt;Overseas Sales Manager&lt;br&gt;Skyfend&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>2025/03/15 10:16</t>
-  </si>
-  <si>
-    <t>Google is a technology company that specializes in internet-related services and products, including search engines, online advertising, cloud computing, software, and hardware. Its primary activity is organizing the world's information and making it universally accessible and useful through its search engine and various other digital services.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Dear John Chen,&lt;/p&gt;
-&lt;p&gt;I hope this message finds you well. We at &lt;strong&gt;Skyfend&lt;/strong&gt;, a subsidiary of Autel, have been closely following Google’s remarkable advancements in technology and innovation. As the Overseas Sales Manager, I am excited to explore potential collaboration opportunities between our companies.&lt;/p&gt;
-&lt;p&gt;Skyfend has established a strong global presence, exporting advanced counter-drone devices to partners across Africa, Europe, and America. Our expertise lies in addressing FPV drone threats and managing commercial drones from leading brands like DJI, Autel, and Parrot. We believe that combining our domain expertise with Google’s technological prowess could unlock significant synergies.&lt;/p&gt;
-&lt;p&gt;Here are a few areas where we see potential for collaboration:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;&lt;strong&gt;AI/ML Integration:&lt;/strong&gt; Leveraging Google’s TensorFlow or Vertex AI to enhance Skyfend’s detection algorithms, reducing false positives and improving real-time threat classification.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Google Cloud for Data Analytics:&lt;/strong&gt; Utilizing BigQuery and Looker for predictive analytics and threat pattern recognition from Skyfend’s sensor data.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Airspace Security with Google Wing:&lt;/strong&gt; Integrating Skyfend’s C-UAS solutions with Project Wing to create safe corridors for delivery drones.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Android/Pixel Integration:&lt;/strong&gt; Embedding Google’s Android OS or Titan M2 chips into Skyfend’s portable devices for enhanced user interfaces and secure communication.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;Geolocation Precision:&lt;/strong&gt; Enhancing Skyfend’s spoofing/jamming accuracy using Google Maps/Earth APIs for real-time terrain and 3D mapping data.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;I would love to discuss these opportunities further. Could we schedule a video meeting or call at your convenience? I have also attached a product brochure for your reference.&lt;/p&gt;
-&lt;p&gt;Looking forward to your response.&lt;/p&gt;
-&lt;p&gt;Best regards,&lt;br&gt;
-Jimmy&lt;br&gt;
-Overseas Sales Manager&lt;br&gt;
-Skyfend&lt;/p&gt;</t>
   </si>
   <si>
     <t>Droniq GmbH</t>
@@ -207,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -215,88 +165,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -663,12 +539,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -694,13 +570,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -708,19 +584,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -728,276 +604,94 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="5"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="4"/>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="5"/>
-      <c r="C48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" t="s">
-        <v>16</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B33:B42"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C33:C42"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C51:C60"/>
-    <mergeCell ref="B51:B60"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>